<commit_message>
Added sort strings to Excel
</commit_message>
<xml_diff>
--- a/HW3Data.xlsx
+++ b/HW3Data.xlsx
@@ -12,7 +12,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Bubble</t>
+  </si>
+  <si>
+    <t>Insertion</t>
+  </si>
+  <si>
+    <t>Selection</t>
+  </si>
+  <si>
+    <t>Merge</t>
+  </si>
+  <si>
+    <t>Quick</t>
+  </si>
+  <si>
+    <t>Shell</t>
+  </si>
+  <si>
+    <t>Arrays.sort()</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,7 +77,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B1:L8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -94,227 +116,248 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" t="n">
-        <v>4668.0</v>
+        <v>4789.0</v>
       </c>
       <c r="C2" t="n">
-        <v>2326.0</v>
+        <v>2478.0</v>
       </c>
       <c r="D2" t="n">
-        <v>8439.0</v>
+        <v>8317.0</v>
       </c>
       <c r="E2" t="n">
-        <v>28753.0</v>
+        <v>28434.0</v>
       </c>
       <c r="F2" t="n">
-        <v>92540.0</v>
+        <v>91841.0</v>
       </c>
       <c r="G2" t="n">
-        <v>317931.0</v>
+        <v>317414.0</v>
       </c>
       <c r="H2" t="n">
-        <v>1172890.0</v>
+        <v>1172677.0</v>
       </c>
       <c r="I2" t="n">
-        <v>5156911.0</v>
+        <v>4879638.0</v>
       </c>
       <c r="J2" t="n">
-        <v>2.4237625E7</v>
+        <v>2.4750065E7</v>
       </c>
       <c r="K2" t="n">
-        <v>1.20888502E8</v>
+        <v>1.2097604E8</v>
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
       <c r="B3" t="n">
-        <v>3634.0</v>
+        <v>3816.0</v>
       </c>
       <c r="C3" t="n">
         <v>1505.0</v>
       </c>
       <c r="D3" t="n">
-        <v>4941.0</v>
+        <v>4652.0</v>
       </c>
       <c r="E3" t="n">
-        <v>17318.0</v>
+        <v>17212.0</v>
       </c>
       <c r="F3" t="n">
-        <v>64167.0</v>
+        <v>64304.0</v>
       </c>
       <c r="G3" t="n">
-        <v>276755.0</v>
+        <v>245325.0</v>
       </c>
       <c r="H3" t="n">
-        <v>1059214.0</v>
+        <v>958934.0</v>
       </c>
       <c r="I3" t="n">
-        <v>3808564.0</v>
+        <v>3793146.0</v>
       </c>
       <c r="J3" t="n">
-        <v>1.512236E7</v>
+        <v>1.5048841E7</v>
       </c>
       <c r="K3" t="n">
-        <v>6.0241653E7</v>
+        <v>6.0182701E7</v>
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
       <c r="B4" t="n">
-        <v>3101.0</v>
+        <v>3542.0</v>
       </c>
       <c r="C4" t="n">
-        <v>1855.0</v>
+        <v>1900.0</v>
       </c>
       <c r="D4" t="n">
-        <v>5306.0</v>
+        <v>5550.0</v>
       </c>
       <c r="E4" t="n">
-        <v>15904.0</v>
+        <v>15859.0</v>
       </c>
       <c r="F4" t="n">
-        <v>48976.0</v>
+        <v>54679.0</v>
       </c>
       <c r="G4" t="n">
-        <v>184564.0</v>
+        <v>161239.0</v>
       </c>
       <c r="H4" t="n">
-        <v>570312.0</v>
+        <v>561097.0</v>
       </c>
       <c r="I4" t="n">
-        <v>2087789.0</v>
+        <v>2091575.0</v>
       </c>
       <c r="J4" t="n">
-        <v>7934999.0</v>
+        <v>7909743.0</v>
       </c>
       <c r="K4" t="n">
-        <v>3.1540228E7</v>
+        <v>3.1530299E7</v>
       </c>
     </row>
     <row r="5">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
       <c r="B5" t="n">
-        <v>9184.0</v>
+        <v>9731.0</v>
       </c>
       <c r="C5" t="n">
         <v>2615.0</v>
       </c>
       <c r="D5" t="n">
-        <v>5838.0</v>
+        <v>5215.0</v>
       </c>
       <c r="E5" t="n">
-        <v>11829.0</v>
+        <v>11388.0</v>
       </c>
       <c r="F5" t="n">
-        <v>24663.0</v>
+        <v>24891.0</v>
       </c>
       <c r="G5" t="n">
-        <v>53629.0</v>
+        <v>53523.0</v>
       </c>
       <c r="H5" t="n">
-        <v>104415.0</v>
+        <v>100766.0</v>
       </c>
       <c r="I5" t="n">
-        <v>248062.0</v>
+        <v>245173.0</v>
       </c>
       <c r="J5" t="n">
-        <v>451101.0</v>
+        <v>452302.0</v>
       </c>
       <c r="K5" t="n">
-        <v>946313.0</v>
+        <v>950160.0</v>
       </c>
     </row>
     <row r="6">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
       <c r="B6" t="n">
-        <v>3634.0</v>
+        <v>3466.0</v>
       </c>
       <c r="C6" t="n">
-        <v>2220.0</v>
+        <v>2174.0</v>
       </c>
       <c r="D6" t="n">
-        <v>4500.0</v>
+        <v>4576.0</v>
       </c>
       <c r="E6" t="n">
-        <v>59316.0</v>
+        <v>59575.0</v>
       </c>
       <c r="F6" t="n">
-        <v>11039.0</v>
+        <v>11130.0</v>
       </c>
       <c r="G6" t="n">
-        <v>23401.0</v>
+        <v>23279.0</v>
       </c>
       <c r="H6" t="n">
-        <v>49281.0</v>
+        <v>49828.0</v>
       </c>
       <c r="I6" t="n">
-        <v>115272.0</v>
+        <v>114102.0</v>
       </c>
       <c r="J6" t="n">
-        <v>295883.0</v>
+        <v>303243.0</v>
       </c>
       <c r="K6" t="n">
-        <v>869160.0</v>
+        <v>868628.0</v>
       </c>
     </row>
     <row r="7">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
       <c r="B7" t="n">
-        <v>2965.0</v>
+        <v>2676.0</v>
       </c>
       <c r="C7" t="n">
         <v>1216.0</v>
       </c>
       <c r="D7" t="n">
-        <v>3071.0</v>
+        <v>3025.0</v>
       </c>
       <c r="E7" t="n">
-        <v>7161.0</v>
+        <v>7009.0</v>
       </c>
       <c r="F7" t="n">
-        <v>16528.0</v>
+        <v>16604.0</v>
       </c>
       <c r="G7" t="n">
-        <v>38713.0</v>
+        <v>38454.0</v>
       </c>
       <c r="H7" t="n">
-        <v>89788.0</v>
+        <v>89818.0</v>
       </c>
       <c r="I7" t="n">
-        <v>207144.0</v>
+        <v>206368.0</v>
       </c>
       <c r="J7" t="n">
-        <v>474912.0</v>
+        <v>474350.0</v>
       </c>
       <c r="K7" t="n">
-        <v>1058849.0</v>
+        <v>1069280.0</v>
       </c>
     </row>
     <row r="8">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
       <c r="B8" t="n">
-        <v>9412.0</v>
+        <v>9564.0</v>
       </c>
       <c r="C8" t="n">
-        <v>7024.0</v>
+        <v>6918.0</v>
       </c>
       <c r="D8" t="n">
-        <v>2143.0</v>
+        <v>2265.0</v>
       </c>
       <c r="E8" t="n">
-        <v>3968.0</v>
+        <v>3999.0</v>
       </c>
       <c r="F8" t="n">
-        <v>14551.0</v>
+        <v>14369.0</v>
       </c>
       <c r="G8" t="n">
-        <v>20603.0</v>
+        <v>20132.0</v>
       </c>
       <c r="H8" t="n">
-        <v>39929.0</v>
+        <v>38758.0</v>
       </c>
       <c r="I8" t="n">
-        <v>69930.0</v>
+        <v>69884.0</v>
       </c>
       <c r="J8" t="n">
-        <v>132257.0</v>
+        <v>131938.0</v>
       </c>
       <c r="K8" t="n">
-        <v>254798.0</v>
+        <v>256166.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto resize the cells
</commit_message>
<xml_diff>
--- a/HW3Data.xlsx
+++ b/HW3Data.xlsx
@@ -82,6 +82,18 @@
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="2" max="2" width="6.609375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="5.49609375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="5.49609375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="6.609375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="6.609375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="7.7265625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="8.83984375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="8.83984375" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="9.95703125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="11.0703125" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="B1" t="n">
@@ -123,31 +135,31 @@
         <v>4789.0</v>
       </c>
       <c r="C2" t="n">
-        <v>2478.0</v>
+        <v>2402.0</v>
       </c>
       <c r="D2" t="n">
-        <v>8317.0</v>
+        <v>8819.0</v>
       </c>
       <c r="E2" t="n">
-        <v>28434.0</v>
+        <v>29437.0</v>
       </c>
       <c r="F2" t="n">
-        <v>91841.0</v>
+        <v>93042.0</v>
       </c>
       <c r="G2" t="n">
-        <v>317414.0</v>
+        <v>319452.0</v>
       </c>
       <c r="H2" t="n">
-        <v>1172677.0</v>
+        <v>1181466.0</v>
       </c>
       <c r="I2" t="n">
-        <v>4879638.0</v>
+        <v>4914718.0</v>
       </c>
       <c r="J2" t="n">
-        <v>2.4750065E7</v>
+        <v>2.4342406E7</v>
       </c>
       <c r="K2" t="n">
-        <v>1.2097604E8</v>
+        <v>1.21826711E8</v>
       </c>
     </row>
     <row r="3">
@@ -155,34 +167,34 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>3816.0</v>
+        <v>4500.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1505.0</v>
+        <v>1550.0</v>
       </c>
       <c r="D3" t="n">
-        <v>4652.0</v>
+        <v>5169.0</v>
       </c>
       <c r="E3" t="n">
-        <v>17212.0</v>
+        <v>17455.0</v>
       </c>
       <c r="F3" t="n">
-        <v>64304.0</v>
+        <v>63665.0</v>
       </c>
       <c r="G3" t="n">
-        <v>245325.0</v>
+        <v>245750.0</v>
       </c>
       <c r="H3" t="n">
-        <v>958934.0</v>
+        <v>959983.0</v>
       </c>
       <c r="I3" t="n">
-        <v>3793146.0</v>
+        <v>3838458.0</v>
       </c>
       <c r="J3" t="n">
-        <v>1.5048841E7</v>
+        <v>1.529035E7</v>
       </c>
       <c r="K3" t="n">
-        <v>6.0182701E7</v>
+        <v>6.0857794E7</v>
       </c>
     </row>
     <row r="4">
@@ -190,34 +202,34 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>3542.0</v>
+        <v>3846.0</v>
       </c>
       <c r="C4" t="n">
         <v>1900.0</v>
       </c>
       <c r="D4" t="n">
-        <v>5550.0</v>
+        <v>5504.0</v>
       </c>
       <c r="E4" t="n">
-        <v>15859.0</v>
+        <v>16011.0</v>
       </c>
       <c r="F4" t="n">
-        <v>54679.0</v>
+        <v>48642.0</v>
       </c>
       <c r="G4" t="n">
-        <v>161239.0</v>
+        <v>163337.0</v>
       </c>
       <c r="H4" t="n">
-        <v>561097.0</v>
+        <v>558634.0</v>
       </c>
       <c r="I4" t="n">
-        <v>2091575.0</v>
+        <v>2475179.0</v>
       </c>
       <c r="J4" t="n">
-        <v>7909743.0</v>
+        <v>7919794.0</v>
       </c>
       <c r="K4" t="n">
-        <v>3.1530299E7</v>
+        <v>3.2799106E7</v>
       </c>
     </row>
     <row r="5">
@@ -225,34 +237,34 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>9731.0</v>
+        <v>14992.0</v>
       </c>
       <c r="C5" t="n">
-        <v>2615.0</v>
+        <v>2813.0</v>
       </c>
       <c r="D5" t="n">
-        <v>5215.0</v>
+        <v>5610.0</v>
       </c>
       <c r="E5" t="n">
-        <v>11388.0</v>
+        <v>12194.0</v>
       </c>
       <c r="F5" t="n">
-        <v>24891.0</v>
+        <v>26579.0</v>
       </c>
       <c r="G5" t="n">
-        <v>53523.0</v>
+        <v>54709.0</v>
       </c>
       <c r="H5" t="n">
-        <v>100766.0</v>
+        <v>99520.0</v>
       </c>
       <c r="I5" t="n">
-        <v>245173.0</v>
+        <v>245188.0</v>
       </c>
       <c r="J5" t="n">
-        <v>452302.0</v>
+        <v>454233.0</v>
       </c>
       <c r="K5" t="n">
-        <v>950160.0</v>
+        <v>944549.0</v>
       </c>
     </row>
     <row r="6">
@@ -260,34 +272,34 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>3466.0</v>
+        <v>5093.0</v>
       </c>
       <c r="C6" t="n">
-        <v>2174.0</v>
+        <v>2250.0</v>
       </c>
       <c r="D6" t="n">
-        <v>4576.0</v>
+        <v>4683.0</v>
       </c>
       <c r="E6" t="n">
-        <v>59575.0</v>
+        <v>60472.0</v>
       </c>
       <c r="F6" t="n">
-        <v>11130.0</v>
+        <v>11388.0</v>
       </c>
       <c r="G6" t="n">
-        <v>23279.0</v>
+        <v>23249.0</v>
       </c>
       <c r="H6" t="n">
-        <v>49828.0</v>
+        <v>49463.0</v>
       </c>
       <c r="I6" t="n">
-        <v>114102.0</v>
+        <v>116139.0</v>
       </c>
       <c r="J6" t="n">
-        <v>303243.0</v>
+        <v>297677.0</v>
       </c>
       <c r="K6" t="n">
-        <v>868628.0</v>
+        <v>861938.0</v>
       </c>
     </row>
     <row r="7">
@@ -295,34 +307,34 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>2676.0</v>
+        <v>3664.0</v>
       </c>
       <c r="C7" t="n">
-        <v>1216.0</v>
+        <v>1307.0</v>
       </c>
       <c r="D7" t="n">
-        <v>3025.0</v>
+        <v>2980.0</v>
       </c>
       <c r="E7" t="n">
-        <v>7009.0</v>
+        <v>7101.0</v>
       </c>
       <c r="F7" t="n">
-        <v>16604.0</v>
+        <v>16786.0</v>
       </c>
       <c r="G7" t="n">
-        <v>38454.0</v>
+        <v>38789.0</v>
       </c>
       <c r="H7" t="n">
-        <v>89818.0</v>
+        <v>89651.0</v>
       </c>
       <c r="I7" t="n">
-        <v>206368.0</v>
+        <v>209379.0</v>
       </c>
       <c r="J7" t="n">
-        <v>474350.0</v>
+        <v>466702.0</v>
       </c>
       <c r="K7" t="n">
-        <v>1069280.0</v>
+        <v>1062225.0</v>
       </c>
     </row>
     <row r="8">
@@ -330,34 +342,34 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>9564.0</v>
+        <v>14962.0</v>
       </c>
       <c r="C8" t="n">
-        <v>6918.0</v>
+        <v>6872.0</v>
       </c>
       <c r="D8" t="n">
-        <v>2265.0</v>
+        <v>2326.0</v>
       </c>
       <c r="E8" t="n">
-        <v>3999.0</v>
+        <v>3938.0</v>
       </c>
       <c r="F8" t="n">
-        <v>14369.0</v>
+        <v>15844.0</v>
       </c>
       <c r="G8" t="n">
-        <v>20132.0</v>
+        <v>20223.0</v>
       </c>
       <c r="H8" t="n">
-        <v>38758.0</v>
+        <v>38698.0</v>
       </c>
       <c r="I8" t="n">
-        <v>69884.0</v>
+        <v>69732.0</v>
       </c>
       <c r="J8" t="n">
-        <v>131938.0</v>
+        <v>132014.0</v>
       </c>
       <c r="K8" t="n">
-        <v>256166.0</v>
+        <v>257079.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed weird init issue
</commit_message>
<xml_diff>
--- a/HW3Data.xlsx
+++ b/HW3Data.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>n</t>
+  </si>
   <si>
     <t>Bubble</t>
   </si>
@@ -83,293 +86,297 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
+    <col min="1" max="1" width="12.16796875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="6.609375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="5.49609375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="5.49609375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="6.609375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="6.609375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="7.7265625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="8.83984375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="6.609375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="7.7265625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="8.83984375" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="9.95703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="11.0703125" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="8.83984375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="9.95703125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C1" t="n">
         <v>20.0</v>
       </c>
-      <c r="C1" t="n">
+      <c r="D1" t="n">
         <v>40.0</v>
       </c>
-      <c r="D1" t="n">
+      <c r="E1" t="n">
         <v>80.0</v>
       </c>
-      <c r="E1" t="n">
+      <c r="F1" t="n">
         <v>160.0</v>
       </c>
-      <c r="F1" t="n">
+      <c r="G1" t="n">
         <v>320.0</v>
       </c>
-      <c r="G1" t="n">
+      <c r="H1" t="n">
         <v>640.0</v>
       </c>
-      <c r="H1" t="n">
+      <c r="I1" t="n">
         <v>1280.0</v>
       </c>
-      <c r="I1" t="n">
+      <c r="J1" t="n">
         <v>2560.0</v>
       </c>
-      <c r="J1" t="n">
+      <c r="K1" t="n">
         <v>5120.0</v>
-      </c>
-      <c r="K1" t="n">
-        <v>10240.0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>4789.0</v>
+        <v>1398.0</v>
       </c>
       <c r="C2" t="n">
-        <v>2402.0</v>
+        <v>5048.0</v>
       </c>
       <c r="D2" t="n">
-        <v>8819.0</v>
+        <v>2615.0</v>
       </c>
       <c r="E2" t="n">
-        <v>29437.0</v>
+        <v>8408.0</v>
       </c>
       <c r="F2" t="n">
-        <v>93042.0</v>
+        <v>28875.0</v>
       </c>
       <c r="G2" t="n">
-        <v>319452.0</v>
+        <v>94608.0</v>
       </c>
       <c r="H2" t="n">
-        <v>1181466.0</v>
+        <v>329046.0</v>
       </c>
       <c r="I2" t="n">
-        <v>4914718.0</v>
+        <v>1173772.0</v>
       </c>
       <c r="J2" t="n">
-        <v>2.4342406E7</v>
+        <v>5058714.0</v>
       </c>
       <c r="K2" t="n">
-        <v>1.21826711E8</v>
+        <v>2.4318746E7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>4500.0</v>
+        <v>1277.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1550.0</v>
+        <v>4181.0</v>
       </c>
       <c r="D3" t="n">
-        <v>5169.0</v>
+        <v>1566.0</v>
       </c>
       <c r="E3" t="n">
-        <v>17455.0</v>
+        <v>4911.0</v>
       </c>
       <c r="F3" t="n">
-        <v>63665.0</v>
+        <v>17623.0</v>
       </c>
       <c r="G3" t="n">
-        <v>245750.0</v>
+        <v>70553.0</v>
       </c>
       <c r="H3" t="n">
-        <v>959983.0</v>
+        <v>245492.0</v>
       </c>
       <c r="I3" t="n">
-        <v>3838458.0</v>
+        <v>958675.0</v>
       </c>
       <c r="J3" t="n">
-        <v>1.529035E7</v>
+        <v>4015906.0</v>
       </c>
       <c r="K3" t="n">
-        <v>6.0857794E7</v>
+        <v>1.5126253E7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>3846.0</v>
+        <v>1079.0</v>
       </c>
       <c r="C4" t="n">
-        <v>1900.0</v>
+        <v>3877.0</v>
       </c>
       <c r="D4" t="n">
-        <v>5504.0</v>
+        <v>1870.0</v>
       </c>
       <c r="E4" t="n">
-        <v>16011.0</v>
+        <v>60533.0</v>
       </c>
       <c r="F4" t="n">
-        <v>48642.0</v>
+        <v>16558.0</v>
       </c>
       <c r="G4" t="n">
-        <v>163337.0</v>
+        <v>49174.0</v>
       </c>
       <c r="H4" t="n">
-        <v>558634.0</v>
+        <v>160220.0</v>
       </c>
       <c r="I4" t="n">
-        <v>2475179.0</v>
+        <v>582567.0</v>
       </c>
       <c r="J4" t="n">
-        <v>7919794.0</v>
+        <v>2079624.0</v>
       </c>
       <c r="K4" t="n">
-        <v>3.2799106E7</v>
+        <v>7926149.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>14992.0</v>
+        <v>3314.0</v>
       </c>
       <c r="C5" t="n">
-        <v>2813.0</v>
+        <v>2098.0</v>
       </c>
       <c r="D5" t="n">
-        <v>5610.0</v>
+        <v>2432.0</v>
       </c>
       <c r="E5" t="n">
-        <v>12194.0</v>
+        <v>5230.0</v>
       </c>
       <c r="F5" t="n">
-        <v>26579.0</v>
+        <v>11495.0</v>
       </c>
       <c r="G5" t="n">
-        <v>54709.0</v>
+        <v>25864.0</v>
       </c>
       <c r="H5" t="n">
-        <v>99520.0</v>
+        <v>53021.0</v>
       </c>
       <c r="I5" t="n">
-        <v>245188.0</v>
+        <v>100706.0</v>
       </c>
       <c r="J5" t="n">
-        <v>454233.0</v>
+        <v>243424.0</v>
       </c>
       <c r="K5" t="n">
-        <v>944549.0</v>
+        <v>452302.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>5093.0</v>
+        <v>1566.0</v>
       </c>
       <c r="C6" t="n">
-        <v>2250.0</v>
+        <v>5033.0</v>
       </c>
       <c r="D6" t="n">
-        <v>4683.0</v>
+        <v>2265.0</v>
       </c>
       <c r="E6" t="n">
-        <v>60472.0</v>
+        <v>3086.0</v>
       </c>
       <c r="F6" t="n">
-        <v>11388.0</v>
+        <v>5413.0</v>
       </c>
       <c r="G6" t="n">
-        <v>23249.0</v>
+        <v>11176.0</v>
       </c>
       <c r="H6" t="n">
-        <v>49463.0</v>
+        <v>23766.0</v>
       </c>
       <c r="I6" t="n">
-        <v>116139.0</v>
+        <v>50360.0</v>
       </c>
       <c r="J6" t="n">
-        <v>297677.0</v>
+        <v>112976.0</v>
       </c>
       <c r="K6" t="n">
-        <v>861938.0</v>
+        <v>297662.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>3664.0</v>
+        <v>1110.0</v>
       </c>
       <c r="C7" t="n">
-        <v>1307.0</v>
+        <v>3010.0</v>
       </c>
       <c r="D7" t="n">
-        <v>2980.0</v>
+        <v>1277.0</v>
       </c>
       <c r="E7" t="n">
-        <v>7101.0</v>
+        <v>3086.0</v>
       </c>
       <c r="F7" t="n">
-        <v>16786.0</v>
+        <v>7207.0</v>
       </c>
       <c r="G7" t="n">
-        <v>38789.0</v>
+        <v>16650.0</v>
       </c>
       <c r="H7" t="n">
-        <v>89651.0</v>
+        <v>38272.0</v>
       </c>
       <c r="I7" t="n">
-        <v>209379.0</v>
+        <v>89894.0</v>
       </c>
       <c r="J7" t="n">
-        <v>466702.0</v>
+        <v>254235.0</v>
       </c>
       <c r="K7" t="n">
-        <v>1062225.0</v>
+        <v>470609.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>14962.0</v>
+        <v>10065.0</v>
       </c>
       <c r="C8" t="n">
-        <v>6872.0</v>
+        <v>2128.0</v>
       </c>
       <c r="D8" t="n">
-        <v>2326.0</v>
+        <v>7100.0</v>
       </c>
       <c r="E8" t="n">
-        <v>3938.0</v>
+        <v>2296.0</v>
       </c>
       <c r="F8" t="n">
-        <v>15844.0</v>
+        <v>3999.0</v>
       </c>
       <c r="G8" t="n">
+        <v>19037.0</v>
+      </c>
+      <c r="H8" t="n">
         <v>20223.0</v>
       </c>
-      <c r="H8" t="n">
-        <v>38698.0</v>
-      </c>
       <c r="I8" t="n">
-        <v>69732.0</v>
+        <v>38576.0</v>
       </c>
       <c r="J8" t="n">
-        <v>132014.0</v>
+        <v>71237.0</v>
       </c>
       <c r="K8" t="n">
-        <v>257079.0</v>
+        <v>132105.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>